<commit_message>
Voltage and current readouts added to gui
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="71">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -198,6 +198,36 @@
   </si>
   <si>
     <t xml:space="preserve">12&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1573,9 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -1708,7 +1740,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -1725,7 +1757,75 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on gui
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="92">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -228,6 +228,69 @@
   </si>
   <si>
     <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD_Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123.123&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperatureUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elapsed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elapsed:</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1639,9 @@
       <c r="G7" t="s">
         <v>63</v>
       </c>
-      <c r="H7"/>
+      <c r="H7" t="s">
+        <v>87</v>
+      </c>
       <c r="I7"/>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
@@ -1596,6 +1661,27 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1740,7 +1826,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -1826,6 +1912,159 @@
       </c>
       <c r="F10" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fan duty cycle added to gui
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2269" uniqueCount="104">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -291,6 +291,42 @@
   </si>
   <si>
     <t xml:space="preserve">Elapsed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fanDutyCycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fanDutyCycleUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp.</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2049,7 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17">
@@ -2065,6 +2101,142 @@
       </c>
       <c r="F19" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial touch pad code
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6279" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7653" uniqueCount="169">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -477,6 +477,51 @@
   </si>
   <si>
     <t xml:space="preserve">4234.234&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.250&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.1&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2178,7 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -2430,10 +2475,10 @@
         <v>146</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
         <v>44</v>
@@ -2459,16 +2504,176 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="41"/>
     <row r="42"/>
     <row r="43"/>

</xml_diff>

<commit_message>
More interactions in gui
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7653" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9243" uniqueCount="180">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -522,6 +522,39 @@
   </si>
   <si>
     <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset timer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2137,7 @@
         <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -2325,7 +2358,7 @@
         <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
         <v>44</v>
@@ -2674,10 +2707,74 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>179</v>
+      </c>
+    </row>
     <row r="45"/>
     <row r="46"/>
   </sheetData>

</xml_diff>

<commit_message>
CPU set to 32MHz, RTC set up to use HSE
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9243" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9515" uniqueCount="183">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -555,6 +555,15 @@
   </si>
   <si>
     <t xml:space="preserve">Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable</t>
   </si>
 </sst>
 </file>
@@ -2636,7 +2645,7 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37">
@@ -2687,7 +2696,7 @@
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40">
@@ -2772,7 +2781,7 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45"/>

</xml_diff>

<commit_message>
Fan RPM measurement added
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9515" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10031" uniqueCount="190">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -564,6 +564,27 @@
   </si>
   <si>
     <t xml:space="preserve">Enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD_Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">012346789.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltageCurrent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage / Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.4</t>
   </si>
 </sst>
 </file>
@@ -1901,7 +1922,7 @@
         <v>59</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1912,9 +1933,7 @@
       <c r="G7" t="s">
         <v>104</v>
       </c>
-      <c r="H7" t="s">
-        <v>87</v>
-      </c>
+      <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
@@ -2006,6 +2025,29 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>184</v>
+      </c>
+      <c r="H10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -2126,7 +2168,7 @@
         <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
         <v>56</v>
@@ -2160,7 +2202,7 @@
         <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
@@ -2211,7 +2253,7 @@
         <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>183</v>
       </c>
       <c r="D11" t="s">
         <v>56</v>
@@ -2293,10 +2335,10 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -2305,32 +2347,32 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -2339,66 +2381,66 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>43</v>
@@ -2407,32 +2449,32 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
@@ -2441,83 +2483,83 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -2526,32 +2568,32 @@
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
         <v>43</v>
@@ -2560,46 +2602,46 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -2611,179 +2653,131 @@
         <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>52</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s">
         <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E39" t="s">
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="s">
-        <v>176</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" t="s">
-        <v>147</v>
-      </c>
-      <c r="E42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F42" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="s">
-        <v>177</v>
-      </c>
-      <c r="C43" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" t="s">
-        <v>43</v>
-      </c>
-      <c r="E43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="s">
-        <v>178</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" t="s">
-        <v>182</v>
-      </c>
-    </row>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
     <row r="45"/>
     <row r="46"/>
   </sheetData>

</xml_diff>

<commit_message>
Better encoder control. Can be used for current limit.
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10031" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10805" uniqueCount="190">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2576,7 +2576,7 @@
         <v>155</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
         <v>147</v>
@@ -2636,7 +2636,7 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>165</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
@@ -2661,7 +2661,7 @@
         <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
Voltage limit can now be edited
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10805" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11327" uniqueCount="192">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t xml:space="preserve">23.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1232&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2772,10 +2778,26 @@
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>191</v>
+      </c>
+    </row>
     <row r="43"/>
     <row r="44"/>
     <row r="45"/>

</xml_diff>

<commit_message>
PID controller added for load
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11327" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11855" uniqueCount="192">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2786,7 +2786,7 @@
         <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="D42" t="s">
         <v>56</v>
@@ -2795,7 +2795,7 @@
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>191</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43"/>

</xml_diff>

<commit_message>
PID for fan controller
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11855" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12383" uniqueCount="193">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t xml:space="preserve">1232&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23&lt;value&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Storing state in EEPROM
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12923" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13199" uniqueCount="197">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Load 40V/8A max</t>
   </si>
 </sst>
 </file>
@@ -2552,7 +2555,7 @@
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>148</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
Silly hysteresis for fan controller
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14327" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14609" uniqueCount="203">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2343,7 +2343,7 @@
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -2377,7 +2377,7 @@
         <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Voltage, current and power is now stored as integers
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/ActiveLoadBigMosfets/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14609" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14891" uniqueCount="204">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Load 36V/8A max</t>
   </si>
 </sst>
 </file>
@@ -2573,7 +2576,7 @@
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28">

</xml_diff>